<commit_message>
fix: add lib excel
</commit_message>
<xml_diff>
--- a/newwwww/JavaApplication18/excel/danhsach.xlsx
+++ b/newwwww/JavaApplication18/excel/danhsach.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="14">
   <si>
     <t>MKH</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>dao3333</t>
+  </si>
+  <si>
+    <t>huy</t>
+  </si>
+  <si>
+    <t>23/04/2024</t>
   </si>
 </sst>
 </file>
@@ -92,7 +98,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -265,6 +271,130 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B8" s="0"/>
+      <c r="C8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>8.37002627E8</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H8" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>13.0</v>
+      </c>
+      <c r="B9" s="0"/>
+      <c r="C9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>8.37002627E8</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H9" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>15.0</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>8.37002627E8</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="H10" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>16.0</v>
+      </c>
+      <c r="B11" s="0"/>
+      <c r="C11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F11" t="n" s="0">
+        <v>8.37002627E8</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H11" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="0">
+        <v>17.0</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F12" t="n" s="0">
+        <v>8.37002627E8</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H12" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>